<commit_message>
Home and foreign currency
</commit_message>
<xml_diff>
--- a/templates/Account Payable.xlsx
+++ b/templates/Account Payable.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dellDevonforce\Provar\ErpFinalProject\rsqasampleproj\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dellDevonforce\Provar\ErpFinalProject\rsqasampleproj\rsqasampleproj\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F377A453-4314-4D7D-90C7-5DF5E4029147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28823EAE-BB28-465D-8214-D2C68D863DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B6C21A89-21B4-4624-A955-66D166717697}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{B6C21A89-21B4-4624-A955-66D166717697}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="15" r:id="rId1"/>
+    <sheet name="BankDetail" sheetId="16" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Vendor</t>
   </si>
@@ -49,6 +50,15 @@
   </si>
   <si>
     <t>NPTestAuto (1146)</t>
+  </si>
+  <si>
+    <t>Bank Account</t>
+  </si>
+  <si>
+    <t>a9d41000000012iAAA</t>
+  </si>
+  <si>
+    <t>a9d1K0000004DGVQA2</t>
   </si>
 </sst>
 </file>
@@ -403,7 +413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D721CDB-A9DB-40A7-92FA-BE728EC43FA8}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -441,4 +451,38 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED581F5-27B1-42C4-BD3E-B23B453B4E89}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>